<commit_message>
Vectors review with Excel
</commit_message>
<xml_diff>
--- a/6_Robotics/Vectors/Vectors.xlsx
+++ b/6_Robotics/Vectors/Vectors.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\6_Robotics\Vectors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB56D4CC-4493-4787-A71A-2EF734C5D422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BEFB4AB8-46B2-4D36-AF54-8C400EF49FEA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="angles" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t xml:space="preserve">a = </t>
   </si>
@@ -59,13 +59,40 @@
   </si>
   <si>
     <t>3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">theta = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">y = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">x = </t>
+  </si>
+  <si>
+    <t>Dot Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R = </t>
+  </si>
+  <si>
+    <t>(dot product is scalar number)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,8 +142,50 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,6 +216,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -157,10 +238,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -189,8 +271,28 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -502,11 +604,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8DFD504-68E3-472F-8409-FCED07A77F6E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -659,4 +761,108 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="10">
+        <f>ATAN(C3/C4)*(180/PI())</f>
+        <v>33.690067525979785</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="B10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="16">
+        <v>3</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="16">
+        <v>-1</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="15">
+        <f>C10*E10+C11*E11</f>
+        <v>1</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+    </row>
+    <row r="11" spans="2:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="B11" s="14"/>
+      <c r="C11" s="16">
+        <v>2</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="16">
+        <v>2</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Vector projects still need more work
</commit_message>
<xml_diff>
--- a/6_Robotics/Vectors/Vectors.xlsx
+++ b/6_Robotics/Vectors/Vectors.xlsx
@@ -768,7 +768,7 @@
   <dimension ref="B3:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -813,20 +813,20 @@
         <v>12</v>
       </c>
       <c r="C10" s="16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="16">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F10" s="18" t="s">
         <v>14</v>
       </c>
       <c r="G10" s="15">
         <f>C10*E10+C11*E11</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -840,7 +840,7 @@
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>

</xml_diff>

<commit_message>
Vector reviews along with projections
</commit_message>
<xml_diff>
--- a/6_Robotics/Vectors/Vectors.xlsx
+++ b/6_Robotics/Vectors/Vectors.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\6_Robotics\Vectors\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5803E92E-F471-4EDE-8F9C-5659C7A630CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="angles" sheetId="2" r:id="rId2"/>
+    <sheet name="Projection" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t xml:space="preserve">a = </t>
   </si>
@@ -79,20 +80,47 @@
     <t xml:space="preserve">B = </t>
   </si>
   <si>
-    <t xml:space="preserve">R = </t>
-  </si>
-  <si>
     <t>(dot product is scalar number)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">| A | = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">| B | = </t>
+  </si>
+  <si>
+    <t>A . B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theta = </t>
+  </si>
+  <si>
+    <t>Acos(A . B / |A| |B|)</t>
+  </si>
+  <si>
+    <t>Projection of A over B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proj = </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = (A . B ) / (|B| |B|) * B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A mag</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B mag</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +209,34 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF0070C0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -224,12 +280,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -237,12 +293,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -271,23 +342,34 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="17" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -604,11 +686,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -704,7 +786,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C10" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F10" s="5">
         <v>-1</v>
@@ -764,102 +846,167 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
+    <row r="2" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="11">
+        <v>3</v>
+      </c>
+    </row>
     <row r="3" spans="2:11" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="11">
+        <f>SQRT(10)</f>
+        <v>3.1622776601683795</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="10">
+        <f>ATAN(C2/C3)*(180/PI())</f>
+        <v>43.491519345092001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="F7" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="B8" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="26">
+        <v>1</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="26">
+        <v>1</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+    </row>
+    <row r="9" spans="2:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="B9" s="27"/>
+      <c r="C9" s="26">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="10">
-        <f>ATAN(C3/C4)*(180/PI())</f>
-        <v>33.690067525979785</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="F9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="B10" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="16">
-        <v>1</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="16">
-        <v>1</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="15">
-        <f>C10*E10+C11*E11</f>
-        <v>3</v>
-      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="26">
+        <v>1</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
     </row>
-    <row r="11" spans="2:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="B11" s="14"/>
+    <row r="11" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>15</v>
+      </c>
       <c r="C11" s="16">
-        <v>2</v>
-      </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="16">
-        <v>1</v>
-      </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
+        <f>SQRT(C8^2+C9^2)</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="16">
+        <f>SQRT(E8^2+E9^2)</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="B14" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="18">
+        <f>C8*E8+C9*E9</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B16" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="21">
+        <f>ACOS(C14/(C11*C12))*(180/PI())</f>
+        <v>18.434948822922021</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B18" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="24">
+        <f>(C14/(C12*C12))*E8</f>
+        <v>1.4999999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="14"/>
+      <c r="C20" s="24">
+        <f>C14/(C12*C12)*E9</f>
+        <v>1.4999999999999996</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Vectors study - Quiz passed - JS review
</commit_message>
<xml_diff>
--- a/6_Robotics/Vectors/Vectors.xlsx
+++ b/6_Robotics/Vectors/Vectors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\6_Robotics\Vectors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5803E92E-F471-4EDE-8F9C-5659C7A630CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE9E711A-0536-45F3-B26E-B46397E7E1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">a = </t>
   </si>
@@ -47,18 +47,6 @@
     <t xml:space="preserve">c = </t>
   </si>
   <si>
-    <t>q1 = ?</t>
-  </si>
-  <si>
-    <t>q2 = ?</t>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>2D</t>
-  </si>
-  <si>
     <t>3D</t>
   </si>
   <si>
@@ -111,6 +99,21 @@
   </si>
   <si>
     <t xml:space="preserve"> B mag</t>
+  </si>
+  <si>
+    <t>a. b</t>
+  </si>
+  <si>
+    <t>b. c</t>
+  </si>
+  <si>
+    <t>a. c</t>
+  </si>
+  <si>
+    <t>sum-product of vectors</t>
+  </si>
+  <si>
+    <t>0 means they're mutually orthogonal</t>
   </si>
 </sst>
 </file>
@@ -120,7 +123,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,12 +145,6 @@
     <font>
       <sz val="14"/>
       <color rgb="FF002060"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF0070C0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -241,18 +238,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -311,9 +302,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -321,56 +312,53 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -687,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:I15"/>
+  <dimension ref="A3:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -701,142 +689,81 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>3</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="I3" s="4">
         <v>1</v>
       </c>
-      <c r="F3" s="5">
-        <v>1</v>
-      </c>
-      <c r="H3" s="7" t="s">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C4" s="3">
         <v>2</v>
       </c>
-      <c r="I3" s="5">
+      <c r="F4" s="4">
+        <v>-4</v>
+      </c>
+      <c r="I4" s="4">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C5" s="3">
         <v>-1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C4" s="4">
-        <v>2</v>
-      </c>
-      <c r="F4" s="5">
-        <v>-2</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2">
-        <v>-1</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="2">
-        <v>-3</v>
-      </c>
-      <c r="G6" s="8" t="s">
+      <c r="F5" s="4">
         <v>5</v>
       </c>
-      <c r="H6" s="3">
-        <f>C6*F3+I3*F6</f>
-        <v>2</v>
+      <c r="I5" s="4">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H7" s="3">
-        <f>C6*F4+F6*I4</f>
-        <v>2</v>
+      <c r="B7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2">
+        <f>SUMPRODUCT(C3:C5,F3:F5)</f>
+        <v>-10</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2">
+        <f>SUMPRODUCT(F3:F5,I3:I5)</f>
+        <v>70</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="5">
-        <v>2</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" s="5">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C10" s="4">
-        <v>2</v>
-      </c>
-      <c r="F10" s="5">
-        <v>-1</v>
-      </c>
-      <c r="I10" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C11" s="4">
-        <v>1</v>
-      </c>
-      <c r="F11" s="5">
-        <v>1</v>
-      </c>
-      <c r="I11" s="5">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2">
-        <v>-1</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="2">
-        <v>-1</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H13" s="3">
-        <f>C13*F9+I9*F13</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H14" s="3">
-        <f>C13*F10+F13*I10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H15" s="3">
-        <f>C13*F11+F13*I11</f>
-        <v>1</v>
+      <c r="B9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2">
+        <f>SUMPRODUCT(C3:C5,I3:I5)</f>
+        <v>-22</v>
       </c>
     </row>
   </sheetData>
@@ -856,154 +783,154 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="2:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="11">
+      <c r="B2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="11">
+      <c r="B3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9">
         <f>SQRT(10)</f>
         <v>3.1622776601683795</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="10">
+      <c r="B4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="8">
         <f>ATAN(C2/C3)*(180/PI())</f>
         <v>43.491519345092001</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="F7" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="B8" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="24">
+        <v>1</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="24">
+        <v>1</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+    </row>
+    <row r="9" spans="2:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="B9" s="25"/>
+      <c r="C9" s="24">
+        <v>2</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="24">
+        <v>1</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+    </row>
+    <row r="11" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="F7" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="B8" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="26">
-        <v>1</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="26">
-        <v>1</v>
-      </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-    </row>
-    <row r="9" spans="2:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="B9" s="27"/>
-      <c r="C9" s="26">
-        <v>2</v>
-      </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="26">
-        <v>1</v>
-      </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-    </row>
-    <row r="11" spans="2:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="16">
+      <c r="C11" s="14">
         <f>SQRT(C8^2+C9^2)</f>
         <v>2.2360679774997898</v>
       </c>
-      <c r="D11" s="19" t="s">
-        <v>23</v>
+      <c r="D11" s="17" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="16">
+      <c r="B12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="14">
         <f>SQRT(E8^2+E9^2)</f>
         <v>1.4142135623730951</v>
       </c>
-      <c r="D12" s="19" t="s">
-        <v>24</v>
+      <c r="D12" s="17" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="B14" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="18">
+      <c r="B14" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="16">
         <f>C8*E8+C9*E9</f>
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="21">
+      <c r="B16" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="19">
         <f>ACOS(C14/(C11*C12))*(180/PI())</f>
         <v>18.434948822922021</v>
       </c>
-      <c r="E16" s="19" t="s">
-        <v>19</v>
+      <c r="E16" s="17" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="B18" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>22</v>
+      <c r="B18" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="24">
+      <c r="B19" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="22">
         <f>(C14/(C12*C12))*E8</f>
         <v>1.4999999999999996</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="14"/>
-      <c r="C20" s="24">
+      <c r="B20" s="12"/>
+      <c r="C20" s="22">
         <f>C14/(C12*C12)*E9</f>
         <v>1.4999999999999996</v>
       </c>

</xml_diff>